<commit_message>
Configurable Proto buff example added
</commit_message>
<xml_diff>
--- a/rest-db-kafka/src/test/resources/createOrder_API_with_OrderCreated_Event.xlsx
+++ b/rest-db-kafka/src/test/resources/createOrder_API_with_OrderCreated_Event.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA0F09E-991E-438C-9666-0A089D20A763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8270DFA3-E9C7-484C-9FE2-FF35DFD851E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateOrder-OrderCreated-Event" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -82,42 +82,15 @@
     <t xml:space="preserve">  @validate_kafka_message @IncludesByPath</t>
   </si>
   <si>
-    <t>orderservice</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
-    <t>{
-  "customer": {
-    "customerId": 1001,
-    "firstname": "Ronnie",
-    "lastname": "Sander"
-  },
-  "orderDesc": "Order Dell Laptop",
-  "orderStatus": "Started",
-  "purchasedProducts": [
-    {
-      "productId": 901,
-      "productName": "Dell Inspiron 3583 15",
-      "productDesc": "Laptop Intel Celeron – 128GB SSD – 4GB DDR4 – 1.6GHz - Intel UHD Graphics 610 - Windows 10 Home in S Mode - Inspiron 15 3000 Series"
-    }
-  ]
-}</t>
-  </si>
-  <si>
-    <t>orderId=orderNumber</t>
-  </si>
-  <si>
     <t>[orderId]</t>
   </si>
   <si>
     <t>VERIFY_ORDER_CREATED_EVENT</t>
   </si>
   <si>
-    <t>order</t>
-  </si>
-  <si>
     <t>Validate created order event</t>
   </si>
   <si>
@@ -128,19 +101,12 @@
   </si>
   <si>
     <t>StoreResponseVariables</t>
-  </si>
-  <si>
-    <t>orderDesc,orderStatus, customer/customerId:firstname:lastname,orderStatus
-Order Dell Laptop,Started,i~1001:Ronnie:Sander,Started</t>
   </si>
   <si>
     <t>orderNumber,orderDesc,orderStatus, customer/customerId:firstname:lastname,orderStatus
 [orderId],Order Dell Laptop,Started,i~1001:Ronnie:Sander,Started</t>
   </si>
   <si>
-    <t>http://localhost:8800/order/5</t>
-  </si>
-  <si>
     <t>As a user needs to;create order;details;order;user;</t>
   </si>
   <si>
@@ -150,7 +116,16 @@
     <t>CREATE_ORDER</t>
   </si>
   <si>
-    <t>JSONMessageType</t>
+    <t>http://localhost:8800/demo/10/Elan</t>
+  </si>
+  <si>
+    <t>ProtoBuffMessageType</t>
+  </si>
+  <si>
+    <t>order-proto</t>
+  </si>
+  <si>
+    <t>orderservice-proto</t>
   </si>
 </sst>
 </file>
@@ -474,29 +449,29 @@
   </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.27734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="85.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="85.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="85.71875" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="85.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,86 +515,80 @@
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="267.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="L2" s="3"/>
       <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="2">
-        <v>201</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="O2" s="2"/>
       <c r="P2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>

</xml_diff>